<commit_message>
pre-finalized usr read routines
</commit_message>
<xml_diff>
--- a/stochastic_surrogate/user-input.xlsx
+++ b/stochastic_surrogate/user-input.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="251">
   <si>
     <t>PARAMETER</t>
   </si>
@@ -198,13 +198,7 @@
     <t xml:space="preserve"> NCO;NCO;NCO </t>
   </si>
   <si>
-    <t xml:space="preserve">CLASSES SEDIMENT DIAMETERS </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.0005;0.02;0.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLASSES SEDIMENT DENSITY </t>
   </si>
   <si>
     <t xml:space="preserve"> 2680;2680;2680 </t>
@@ -833,12 +827,21 @@
   <si>
     <t>list with 1 element per sed. class - requires CLASSES SEDIMENT DIAMETERS as Indirect Calib. Par !</t>
   </si>
+  <si>
+    <t xml:space="preserve">0.1, 0.024, 0.0085, 0.0023 </t>
+  </si>
+  <si>
+    <t>Cailbration file (calib_pts)</t>
+  </si>
+  <si>
+    <t>/home/data/calibration_points.csv</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -910,8 +913,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -962,6 +973,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor rgb="FF333300"/>
       </patternFill>
     </fill>
@@ -1032,7 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1084,12 +1101,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1133,12 +1144,125 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1189,45 +1313,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1242,7 +1327,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:D63" totalsRowShown="0" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:D63" totalsRowShown="0" headerRowBorderDxfId="8">
   <autoFilter ref="A8:D63"/>
   <sortState ref="A9:C57">
     <sortCondition ref="A8:A57"/>
@@ -1274,11 +1359,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="F13:G15" totalsRowShown="0" dataDxfId="2" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="F13:G15" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="F13:G15"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="RECALCULATION PARAMETERS" dataDxfId="1"/>
-    <tableColumn id="2" name="PARAMETER TO RECALCULATE" dataDxfId="0"/>
+    <tableColumn id="1" name="RECALCULATION PARAMETERS" dataDxfId="5"/>
+    <tableColumn id="2" name="PARAMETER TO RECALCULATE" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1548,38 +1633,38 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="25" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" style="4" customWidth="1"/>
     <col min="5" max="16384" width="11.5703125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+        <v>139</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
@@ -1588,12 +1673,12 @@
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
@@ -1606,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1627,26 +1712,26 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B9" s="22">
         <v>1</v>
@@ -1655,7 +1740,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1664,12 +1749,12 @@
       <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
@@ -1682,7 +1767,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1694,12 +1779,12 @@
         <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B14" s="22">
         <v>15</v>
@@ -1708,12 +1793,12 @@
         <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B15" s="22">
         <v>1000</v>
@@ -1722,12 +1807,12 @@
         <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" s="22">
         <v>10000</v>
@@ -1736,12 +1821,12 @@
         <v>20</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B17" s="22">
         <v>100000</v>
@@ -1750,94 +1835,92 @@
         <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="1:4" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="40" t="s">
-        <v>177</v>
+        <v>65</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
     </row>
-    <row r="22" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="23"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="15" t="s">
+    <row r="22" spans="1:4" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+    </row>
+    <row r="23" spans="1:4" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" s="8" t="str">
-        <f>VLOOKUP(A24,ignore!$A$8:$D$94,4,FALSE)</f>
-        <v>list of float (m/s)</v>
-      </c>
-      <c r="D24" s="4" t="str">
-        <f>VLOOKUP(A24,ignore!$A$8:$C$94,3,FALSE)</f>
-        <v>list with 1 element per sed. class - requires CLASSES SEDIMENT DIAMETERS as Indirect Calib. Par !</v>
+      <c r="D24" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C25" s="8" t="str">
         <f>VLOOKUP(A25,ignore!$A$8:$D$94,4,FALSE)</f>
-        <v>select</v>
+        <v>list of float (m/s)</v>
       </c>
       <c r="D25" s="4" t="str">
         <f>VLOOKUP(A25,ignore!$A$8:$C$94,3,FALSE)</f>
-        <v>Select a Parameter for more information</v>
+        <v>list with 1 element per sed. class - requires CLASSES SEDIMENT DIAMETERS as Indirect Calib. Par !</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C26" s="8" t="str">
         <f>VLOOKUP(A26,ignore!$A$8:$D$94,4,FALSE)</f>
@@ -1850,10 +1933,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C27" s="8" t="str">
         <f>VLOOKUP(A27,ignore!$A$8:$D$94,4,FALSE)</f>
@@ -1864,135 +1947,135 @@
         <v>Select a Parameter for more information</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="8" t="str">
+        <f>VLOOKUP(A28,ignore!$A$8:$D$94,4,FALSE)</f>
+        <v>select</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f>VLOOKUP(A28,ignore!$A$8:$C$94,3,FALSE)</f>
+        <v>Select a Parameter for more information</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="C29" s="15" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="8" t="str">
+        <f>VLOOKUP(A32,ignore!$A$8:$D$94,4,FALSE)</f>
+        <v>select</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <f>VLOOKUP(A32,ignore!$A$8:$C$94,3,FALSE)</f>
+        <v>Select a Parameter for more information</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="27" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="28"/>
+    </row>
+    <row r="34" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="8" t="str">
-        <f>VLOOKUP(A31,ignore!$A$8:$D$94,4,FALSE)</f>
-        <v>select</v>
-      </c>
-      <c r="D31" s="4" t="str">
-        <f>VLOOKUP(A31,ignore!$A$8:$C$94,3,FALSE)</f>
-        <v>Select a Parameter for more information</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="29" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="30"/>
-    </row>
-    <row r="33" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="38" t="s">
+      <c r="D34" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="31" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="31" t="str">
+        <f>IF(ISNUMBER(MATCH($A$32,Table3[RECALCULATION PARAMETERS],0)),VLOOKUP($A$32,Table3[],2),"None")</f>
+        <v>None</v>
+      </c>
+      <c r="B35" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="33" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="str">
-        <f>IF(ISNUMBER(MATCH($A$31,Table3[RECALCULATION PARAMETERS],0)),VLOOKUP($A$31,Table3[],2),"None")</f>
-        <v>None</v>
-      </c>
-      <c r="B34" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="18" t="str">
-        <f>VLOOKUP(A40,ignore!$A$8:$D$94,4)</f>
-        <v>float</v>
-      </c>
-      <c r="D40" s="9" t="str">
-        <f>VLOOKUP(A40,ignore!$A$8:$C$94,3)</f>
-        <v>diffusion and source terms for Spalart-Allmaras equation</v>
-      </c>
+      <c r="A40" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="13"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B41" s="50" t="s">
+        <v>2</v>
       </c>
       <c r="C41" s="18" t="str">
         <f>VLOOKUP(A41,ignore!$A$8:$D$94,4)</f>
-        <v>float (N/m²)</v>
+        <v>float</v>
       </c>
       <c r="D41" s="9" t="str">
         <f>VLOOKUP(A41,ignore!$A$8:$C$94,3)</f>
-        <v>list of floats corresponding to number of sediment classes</v>
+        <v>diffusion and source terms for Spalart-Allmaras equation</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B42" s="50" t="s">
+        <v>4</v>
       </c>
       <c r="C42" s="18" t="str">
         <f>VLOOKUP(A42,ignore!$A$8:$D$94,4)</f>
-        <v>float (g/L)</v>
+        <v>float (N/m²)</v>
       </c>
       <c r="D42" s="9" t="str">
         <f>VLOOKUP(A42,ignore!$A$8:$C$94,3)</f>
@@ -2000,38 +2083,137 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="18" t="str">
+        <f>VLOOKUP(A43,ignore!$A$8:$D$94,4)</f>
+        <v>float (g/L)</v>
+      </c>
+      <c r="D43" s="9" t="str">
+        <f>VLOOKUP(A43,ignore!$A$8:$C$94,3)</f>
+        <v>list of floats corresponding to number of sediment classes</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B44" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="19" t="str">
-        <f>VLOOKUP(A43,ignore!$A$8:$D$94,4)</f>
+      <c r="C44" s="19" t="str">
+        <f>VLOOKUP(A44,ignore!$A$8:$D$94,4)</f>
         <v>float</v>
       </c>
-      <c r="D43" s="10" t="str">
-        <f>VLOOKUP(A43,ignore!$A$8:$C$94,3)</f>
+      <c r="D44" s="10" t="str">
+        <f>VLOOKUP(A44,ignore!$A$8:$C$94,3)</f>
         <v>diffusion and source terms for Spalart-Allmaras equation</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="42" t="s">
+        <v>246</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="C48" s="44" t="str">
+        <f>VLOOKUP(A48,ignore!$A$8:$D$94,4,FALSE)</f>
+        <v>list of float (m)</v>
+      </c>
+      <c r="D48" s="45" t="str">
+        <f>VLOOKUP(A48,ignore!$A$8:$C$94,3,FALSE)</f>
+        <v>list with one element per sediment class</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="31" t="str">
+        <f>IF(ISNUMBER(MATCH($A$48,Table3[RECALCULATION PARAMETERS],0)),VLOOKUP($A$48,Table3[],2),"None")</f>
+        <v>CLASSES SETTLING VELOCITIES</v>
+      </c>
+      <c r="B51" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="53" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A11:D11"/>
   </mergeCells>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="A35">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
       <formula>"None"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>IF($A$34="None",FALSE,TRUE)</formula>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>IF($A$35="None",FALSE,TRUE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>"None"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF($A$35="None",FALSE,TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2053,7 +2235,7 @@
           <x14:formula1>
             <xm:f>ignore!$A$8:$A$94</xm:f>
           </x14:formula1>
-          <xm:sqref>A24:A27 A40:A43 A31</xm:sqref>
+          <xm:sqref>A25:A28 A41:A44 A32 A48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2065,7 +2247,7 @@
           <x14:formula1>
             <xm:f>ignore!$C$4:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B34</xm:sqref>
+          <xm:sqref>B35 B51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2078,8 +2260,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2101,7 +2283,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2122,24 +2304,24 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>153</v>
+      <c r="F8" s="26" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" s="2">
         <v>1E-4</v>
@@ -2148,15 +2330,15 @@
         <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" s="2">
         <v>9.9999999999999995E-7</v>
@@ -2165,15 +2347,15 @@
         <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2">
         <v>9.9999999999999995E-7</v>
@@ -2182,15 +2364,15 @@
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2">
         <v>9.9999999999999995E-7</v>
@@ -2199,29 +2381,29 @@
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -2230,18 +2412,18 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -2250,32 +2432,32 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="G15" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B16">
         <v>0.9</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -2284,54 +2466,54 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B19">
         <v>0.1</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B20">
         <v>0.03</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B21">
         <v>0.6</v>
@@ -2340,12 +2522,12 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B22">
         <v>0.55000000000000004</v>
@@ -2354,12 +2536,12 @@
         <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2373,7 +2555,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B24">
         <v>0.55000000000000004</v>
@@ -2382,26 +2564,26 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
@@ -2410,12 +2592,12 @@
         <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2424,18 +2606,18 @@
         <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B28">
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
@@ -2443,21 +2625,21 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2466,12 +2648,12 @@
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2480,12 +2662,12 @@
         <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2494,12 +2676,12 @@
         <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2508,12 +2690,12 @@
         <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -2527,7 +2709,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B35">
         <v>60</v>
@@ -2541,7 +2723,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B36">
         <v>50</v>
@@ -2555,7 +2737,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B37">
         <v>200</v>
@@ -2569,13 +2751,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B38">
         <v>8000</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
@@ -2583,13 +2765,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
@@ -2597,55 +2779,55 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B43">
         <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
@@ -2653,13 +2835,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B44">
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
@@ -2667,13 +2849,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B45">
         <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
@@ -2681,13 +2863,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
@@ -2695,13 +2877,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
@@ -2709,13 +2891,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D48" t="s">
         <v>20</v>
@@ -2723,7 +2905,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B49" s="2">
         <v>1E-4</v>
@@ -2732,68 +2914,68 @@
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B50" s="2">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B52" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B53" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B54" t="s">
         <v>28</v>
@@ -2802,12 +2984,12 @@
         <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B55" t="s">
         <v>23</v>
@@ -2816,12 +2998,12 @@
         <v>27</v>
       </c>
       <c r="D55" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B56" t="s">
         <v>36</v>
@@ -2830,32 +3012,32 @@
         <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B57" t="s">
         <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D57" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
@@ -2863,7 +3045,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -2877,7 +3059,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -2891,13 +3073,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D61" t="s">
         <v>20</v>
@@ -2905,7 +3087,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B62" t="s">
         <v>23</v>
@@ -2914,32 +3096,32 @@
         <v>26</v>
       </c>
       <c r="D62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B63" t="s">
         <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D63" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>19</v>
@@ -2947,41 +3129,41 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B65">
         <v>0.3</v>
       </c>
       <c r="C65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B66" t="s">
         <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
@@ -2989,16 +3171,16 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B68">
         <v>1.3</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D68" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -3009,38 +3191,38 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D69" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D70" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D71" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -3051,77 +3233,77 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D72" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B74" t="s">
         <v>56</v>
       </c>
       <c r="C74" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D74" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" t="s">
+        <v>129</v>
+      </c>
+      <c r="C75" t="s">
         <v>130</v>
       </c>
-      <c r="B75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C75" t="s">
-        <v>132</v>
-      </c>
       <c r="D75" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B76" t="s">
         <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D77" t="s">
         <v>20</v>
@@ -3129,13 +3311,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D78" t="s">
         <v>20</v>
@@ -3149,24 +3331,24 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D79" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B80">
         <v>1.5</v>
       </c>
       <c r="C80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D80" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -3177,49 +3359,49 @@
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D81" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B82" s="2">
         <v>1E-3</v>
       </c>
       <c r="C82" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D82" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B83">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B84">
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D84" t="s">
         <v>20</v>
@@ -3227,41 +3409,41 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B85" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C85" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D85" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B86">
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D86" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B87">
         <v>14</v>
       </c>
       <c r="C87" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D87" t="s">
         <v>20</v>
@@ -3269,13 +3451,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B88">
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D88" t="s">
         <v>20</v>
@@ -3283,41 +3465,41 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B89" t="s">
         <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D89" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B90">
         <v>0.8</v>
       </c>
       <c r="C90" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D90" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D91" t="s">
         <v>20</v>
@@ -3325,41 +3507,41 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D92" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D93" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D94" t="s">
         <v>20</v>

</xml_diff>